<commit_message>
default equipments for container, position amount (addes SQL script)
</commit_message>
<xml_diff>
--- a/ContainerStar/ContainerStar/Generation/ContainerStar.Generation/Declarations/Stammdaten.xlsx
+++ b/ContainerStar/ContainerStar/Generation/ContainerStar.Generation/Declarations/Stammdaten.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="156" windowWidth="19092" windowHeight="8412" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="213">
   <si>
     <t>Schema</t>
   </si>
@@ -1217,40 +1217,40 @@
   <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W12" sqref="W12"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="46.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="11.5546875" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" customWidth="1"/>
-    <col min="13" max="13" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="55" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="53.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.44140625" customWidth="1"/>
-    <col min="19" max="19" width="66.5546875" style="7" customWidth="1"/>
-    <col min="20" max="20" width="25.44140625" customWidth="1"/>
-    <col min="21" max="21" width="21.88671875" style="7" customWidth="1"/>
+    <col min="15" max="15" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" customWidth="1"/>
+    <col min="19" max="19" width="66.5703125" style="7" customWidth="1"/>
+    <col min="20" max="20" width="25.42578125" customWidth="1"/>
+    <col min="21" max="21" width="21.85546875" style="7" customWidth="1"/>
     <col min="22" max="22" width="19" style="7" customWidth="1"/>
-    <col min="23" max="23" width="15.33203125" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" customWidth="1"/>
     <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="27" max="27" width="8.88671875" style="14"/>
+    <col min="27" max="27" width="8.85546875" style="14"/>
     <col min="28" max="28" width="32" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="AB11"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="AB13"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="AB15"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -2045,30 +2045,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K23" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.33203125" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="37.44140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="29.6640625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="30.88671875" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
-    <col min="13" max="13" width="27.6640625" customWidth="1"/>
-    <col min="15" max="16" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37.42578125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="15" max="16" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>11</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>11</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>11</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>11</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -4250,14 +4250,14 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="46.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4276,25 +4276,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="46.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4312,6 +4312,17 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -4332,15 +4343,15 @@
       <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="46.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4370,17 +4381,17 @@
       <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4400,7 +4411,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="383" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="383" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:C380"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
invoices v1.0 (+ SQL script)
</commit_message>
<xml_diff>
--- a/ContainerStar/ContainerStar/Generation/ContainerStar.Generation/Declarations/Stammdaten.xlsx
+++ b/ContainerStar/ContainerStar/Generation/ContainerStar.Generation/Declarations/Stammdaten.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="223">
   <si>
     <t>Schema</t>
   </si>
@@ -782,6 +782,36 @@
   </si>
   <si>
     <t>GenerateFilter</t>
+  </si>
+  <si>
+    <t>Rechnung</t>
+  </si>
+  <si>
+    <t>Invoices</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>InvoicePositions</t>
+  </si>
+  <si>
+    <t>invoiceId</t>
+  </si>
+  <si>
+    <t>Rechnungposition</t>
+  </si>
+  <si>
+    <t>Invoice position</t>
+  </si>
+  <si>
+    <t>Settings/InvoicePositions</t>
+  </si>
+  <si>
+    <t>invoicePositions</t>
+  </si>
+  <si>
+    <t>Positionen</t>
   </si>
 </sst>
 </file>
@@ -1214,13 +1244,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD17"/>
+  <dimension ref="A1:AD19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14:B14"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,7 +2023,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -2025,6 +2055,79 @@
         <v>211</v>
       </c>
       <c r="AB17"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O18" t="s">
+        <v>213</v>
+      </c>
+      <c r="P18" t="s">
+        <v>215</v>
+      </c>
+      <c r="R18" t="s">
+        <v>7</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="T18" t="s">
+        <v>221</v>
+      </c>
+      <c r="U18" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="V18" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA18" s="14">
+        <v>12</v>
+      </c>
+      <c r="AB18" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>216</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19" t="s">
+        <v>217</v>
+      </c>
+      <c r="M19" t="s">
+        <v>214</v>
+      </c>
+      <c r="O19" t="s">
+        <v>218</v>
+      </c>
+      <c r="P19" t="s">
+        <v>219</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:P5">
@@ -2045,11 +2148,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O41" sqref="O41"/>
+      <selection pane="bottomRight" activeCell="A72" sqref="A72:I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4278,7 +4381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
add/change order/customer/comm parnter/position fields
</commit_message>
<xml_diff>
--- a/ContainerStar/ContainerStar/Generation/ContainerStar.Generation/Declarations/Stammdaten.xlsx
+++ b/ContainerStar/ContainerStar/Generation/ContainerStar.Generation/Declarations/Stammdaten.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="8415" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tables{T}" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">Drl or AsPro
 </t>
@@ -65,7 +66,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">Skip constructor generation
 </t>
@@ -90,7 +92,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Skip controller generation</t>
         </r>
@@ -103,7 +106,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">Skip constructor generation
 </t>
@@ -118,7 +122,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Add execution of ExtraEntityToModel implemented in partial custom part of controller</t>
         </r>
@@ -132,7 +137,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Add execution of ExtraModelToEntity implemented in partial custom part of controller</t>
         </r>
@@ -143,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="244">
   <si>
     <t>Schema</t>
   </si>
@@ -541,18 +547,6 @@
     <t>City</t>
   </si>
   <si>
-    <t>Rechnung mit MwSt.</t>
-  </si>
-  <si>
-    <t>Automat. Abbuchung</t>
-  </si>
-  <si>
-    <t>Automat. Rabatt in %</t>
-  </si>
-  <si>
-    <t>Automat. Rechnung</t>
-  </si>
-  <si>
     <t>Land</t>
   </si>
   <si>
@@ -848,6 +842,45 @@
   </si>
   <si>
     <t>Transport Order</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>BLZ</t>
+  </si>
+  <si>
+    <t>Kreditinstitut</t>
+  </si>
+  <si>
+    <t>Kontonummer</t>
+  </si>
+  <si>
+    <t>Account number</t>
+  </si>
+  <si>
+    <t>IsProspectiveCustomer</t>
+  </si>
+  <si>
+    <t>Is Prospective Customer</t>
+  </si>
+  <si>
+    <t>Interessent</t>
+  </si>
+  <si>
+    <t>MwSt.</t>
+  </si>
+  <si>
+    <t>A. Abbuchung</t>
+  </si>
+  <si>
+    <t>Rabatt in %</t>
+  </si>
+  <si>
+    <t>A. Rechnung</t>
   </si>
 </sst>
 </file>
@@ -876,14 +909,16 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1282,7 +1317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1405,7 +1440,7 @@
         <v>67</v>
       </c>
       <c r="AD1" s="8" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1791,16 +1826,16 @@
         <v>7</v>
       </c>
       <c r="S10" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="T10" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="U10" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="V10" s="7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="AA10" s="14">
         <v>8</v>
@@ -1817,7 +1852,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
         <v>44</v>
@@ -1832,16 +1867,16 @@
         <v>7</v>
       </c>
       <c r="L11" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M11" t="s">
         <v>108</v>
       </c>
       <c r="O11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="P11" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="AB11"/>
     </row>
@@ -1850,7 +1885,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C12" t="s">
         <v>44</v>
@@ -1871,7 +1906,7 @@
         <v>79</v>
       </c>
       <c r="O12" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="P12" t="s">
         <v>81</v>
@@ -1880,16 +1915,16 @@
         <v>7</v>
       </c>
       <c r="S12" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="T12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="U12" s="7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="W12" s="7" t="s">
         <v>27</v>
@@ -1901,7 +1936,7 @@
         <v>9</v>
       </c>
       <c r="AB12" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="AD12" t="s">
         <v>7</v>
@@ -1912,7 +1947,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C13" t="s">
         <v>44</v>
@@ -1927,19 +1962,19 @@
         <v>7</v>
       </c>
       <c r="L13" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="M13" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="N13" t="s">
         <v>79</v>
       </c>
       <c r="O13" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="P13" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AB13"/>
     </row>
@@ -1948,7 +1983,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C14" t="s">
         <v>44</v>
@@ -1960,25 +1995,25 @@
         <v>7</v>
       </c>
       <c r="N14" t="s">
+        <v>171</v>
+      </c>
+      <c r="O14" t="s">
+        <v>172</v>
+      </c>
+      <c r="P14" t="s">
+        <v>172</v>
+      </c>
+      <c r="R14" t="s">
+        <v>7</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="T14" t="s">
         <v>175</v>
       </c>
-      <c r="O14" t="s">
-        <v>176</v>
-      </c>
-      <c r="P14" t="s">
-        <v>176</v>
-      </c>
-      <c r="R14" t="s">
-        <v>7</v>
-      </c>
-      <c r="S14" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="T14" t="s">
-        <v>179</v>
-      </c>
       <c r="U14" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="V14" s="7" t="s">
         <v>79</v>
@@ -1989,7 +2024,7 @@
         <v>10</v>
       </c>
       <c r="AB14" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="AD14" t="s">
         <v>7</v>
@@ -2000,7 +2035,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
         <v>44</v>
@@ -2015,16 +2050,16 @@
         <v>7</v>
       </c>
       <c r="L15" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M15" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="N15" t="s">
         <v>79</v>
       </c>
       <c r="O15" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="P15" t="s">
         <v>79</v>
@@ -2036,7 +2071,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C16" t="s">
         <v>44</v>
@@ -2048,10 +2083,10 @@
         <v>7</v>
       </c>
       <c r="O16" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="P16" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="R16" t="s">
         <v>7</v>
@@ -2062,7 +2097,7 @@
         <v>11</v>
       </c>
       <c r="AB16" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
@@ -2070,7 +2105,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C17" t="s">
         <v>44</v>
@@ -2085,16 +2120,16 @@
         <v>7</v>
       </c>
       <c r="L17" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="M17" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="O17" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="P17" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="AB17"/>
     </row>
@@ -2103,7 +2138,7 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s">
         <v>44</v>
@@ -2112,31 +2147,31 @@
         <v>55</v>
       </c>
       <c r="O18" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="P18" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="R18" t="s">
         <v>7</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="T18" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="U18" s="7" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="AA18" s="14">
         <v>12</v>
       </c>
       <c r="AB18" s="12" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="AD18" t="s">
         <v>7</v>
@@ -2147,7 +2182,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C19" t="s">
         <v>44</v>
@@ -2159,16 +2194,16 @@
         <v>7</v>
       </c>
       <c r="L19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="M19" t="s">
+        <v>210</v>
+      </c>
+      <c r="O19" t="s">
         <v>214</v>
       </c>
-      <c r="O19" t="s">
-        <v>218</v>
-      </c>
       <c r="P19" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
@@ -2176,7 +2211,7 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C20" t="s">
         <v>44</v>
@@ -2185,10 +2220,10 @@
         <v>55</v>
       </c>
       <c r="O20" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="P20" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="R20" t="s">
         <v>7</v>
@@ -2197,7 +2232,7 @@
         <v>13</v>
       </c>
       <c r="AB20" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
@@ -2205,7 +2240,7 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
@@ -2217,10 +2252,10 @@
         <v>7</v>
       </c>
       <c r="O21" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="P21" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="R21" t="s">
         <v>7</v>
@@ -2231,7 +2266,7 @@
         <v>14</v>
       </c>
       <c r="AB21" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
@@ -2239,7 +2274,7 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C22" t="s">
         <v>44</v>
@@ -2254,16 +2289,16 @@
         <v>7</v>
       </c>
       <c r="L22" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="M22" t="s">
+        <v>225</v>
+      </c>
+      <c r="O22" t="s">
         <v>229</v>
       </c>
-      <c r="O22" t="s">
-        <v>233</v>
-      </c>
       <c r="P22" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="AB22"/>
     </row>
@@ -2284,13 +2319,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R72"/>
+  <dimension ref="A1:R76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C64" sqref="C64"/>
+      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3221,13 +3256,13 @@
         <v>7</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>132</v>
+        <v>240</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O30" s="14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P30" s="14">
         <v>1</v>
@@ -3250,13 +3285,13 @@
         <v>7</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>133</v>
+        <v>241</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="O31" s="14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P31" s="14">
         <v>2</v>
@@ -3282,13 +3317,13 @@
         <v>7</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>135</v>
+        <v>243</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="O32" s="14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P32" s="14">
         <v>3</v>
@@ -3311,7 +3346,7 @@
         <v>7</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I33" s="7" t="s">
         <v>117</v>
@@ -3340,7 +3375,7 @@
         <v>7</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I34" s="7" t="s">
         <v>118</v>
@@ -3398,7 +3433,7 @@
         <v>7</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I36" s="7" t="s">
         <v>120</v>
@@ -3433,7 +3468,7 @@
         <v>121</v>
       </c>
       <c r="O37" s="14">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P37" s="14">
         <v>1</v>
@@ -3447,7 +3482,7 @@
         <v>108</v>
       </c>
       <c r="C38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
@@ -3456,16 +3491,16 @@
         <v>7</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O38" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P38" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -3476,7 +3511,7 @@
         <v>108</v>
       </c>
       <c r="C39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
@@ -3485,16 +3520,16 @@
         <v>7</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O39" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P39" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -3505,7 +3540,7 @@
         <v>108</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>231</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -3514,16 +3549,16 @@
         <v>7</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>143</v>
+        <v>234</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>124</v>
+        <v>231</v>
       </c>
       <c r="O40" s="14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P40" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -3534,25 +3569,22 @@
         <v>108</v>
       </c>
       <c r="C41" t="s">
-        <v>125</v>
+        <v>232</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
       </c>
-      <c r="E41" t="s">
-        <v>7</v>
-      </c>
       <c r="F41" t="s">
         <v>7</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>134</v>
+        <v>235</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>140</v>
+        <v>236</v>
       </c>
       <c r="O41" s="14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P41" s="14">
         <v>2</v>
@@ -3566,7 +3598,7 @@
         <v>108</v>
       </c>
       <c r="C42" t="s">
-        <v>126</v>
+        <v>233</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
@@ -3575,10 +3607,10 @@
         <v>7</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>144</v>
+        <v>233</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>144</v>
+        <v>233</v>
       </c>
       <c r="O42" s="14">
         <v>4</v>
@@ -3592,28 +3624,28 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>124</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
       </c>
-      <c r="E43" t="s">
-        <v>7</v>
-      </c>
       <c r="F43" t="s">
         <v>7</v>
       </c>
-      <c r="G43" t="s">
-        <v>7</v>
-      </c>
       <c r="H43" s="7" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>27</v>
+        <v>124</v>
+      </c>
+      <c r="O43" s="14">
+        <v>7</v>
+      </c>
+      <c r="P43" s="14">
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -3621,10 +3653,10 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="C44" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="D44" t="s">
         <v>7</v>
@@ -3635,25 +3667,28 @@
       <c r="F44" t="s">
         <v>7</v>
       </c>
-      <c r="G44" t="s">
-        <v>7</v>
-      </c>
       <c r="H44" s="7" t="s">
-        <v>154</v>
+        <v>242</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="O44" s="14">
+        <v>7</v>
+      </c>
+      <c r="P44" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="C45" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
@@ -3661,25 +3696,28 @@
       <c r="F45" t="s">
         <v>7</v>
       </c>
-      <c r="G45" t="s">
-        <v>7</v>
-      </c>
       <c r="H45" s="7" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="O45" s="14">
+        <v>5</v>
+      </c>
+      <c r="P45" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>118</v>
+        <v>237</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
@@ -3687,17 +3725,11 @@
       <c r="E46" t="s">
         <v>7</v>
       </c>
-      <c r="F46" t="s">
-        <v>7</v>
-      </c>
-      <c r="G46" t="s">
-        <v>7</v>
-      </c>
       <c r="H46" s="7" t="s">
-        <v>141</v>
+        <v>239</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>118</v>
+        <v>238</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -3705,10 +3737,10 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C47" t="s">
-        <v>119</v>
+        <v>27</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -3719,11 +3751,14 @@
       <c r="F47" t="s">
         <v>7</v>
       </c>
+      <c r="G47" t="s">
+        <v>7</v>
+      </c>
       <c r="H47" s="7" t="s">
-        <v>119</v>
+        <v>27</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>119</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -3731,10 +3766,10 @@
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C48" t="s">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
@@ -3745,11 +3780,14 @@
       <c r="F48" t="s">
         <v>7</v>
       </c>
+      <c r="G48" t="s">
+        <v>7</v>
+      </c>
       <c r="H48" s="7" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -3757,25 +3795,25 @@
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C49" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
       </c>
-      <c r="E49" t="s">
-        <v>7</v>
-      </c>
       <c r="F49" t="s">
         <v>7</v>
       </c>
+      <c r="G49" t="s">
+        <v>7</v>
+      </c>
       <c r="H49" s="7" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -3783,10 +3821,10 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="D50" t="s">
         <v>7</v>
@@ -3801,10 +3839,10 @@
         <v>7</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -3812,10 +3850,10 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="C51" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -3827,10 +3865,10 @@
         <v>7</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -3838,25 +3876,25 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="C52" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
       </c>
+      <c r="E52" t="s">
+        <v>7</v>
+      </c>
       <c r="F52" t="s">
         <v>7</v>
       </c>
-      <c r="G52" t="s">
-        <v>7</v>
-      </c>
       <c r="H52" s="7" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -3864,10 +3902,10 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="C53" t="s">
-        <v>167</v>
+        <v>121</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
@@ -3878,17 +3916,11 @@
       <c r="F53" t="s">
         <v>7</v>
       </c>
-      <c r="G53" t="s">
-        <v>7</v>
-      </c>
       <c r="H53" s="7" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="J53" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -3896,10 +3928,10 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C54" t="s">
-        <v>170</v>
+        <v>27</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
@@ -3914,10 +3946,10 @@
         <v>7</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>170</v>
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -3925,10 +3957,10 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="C55" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
@@ -3939,20 +3971,11 @@
       <c r="F55" t="s">
         <v>7</v>
       </c>
-      <c r="G55" t="s">
-        <v>7</v>
-      </c>
       <c r="H55" s="7" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="O55" s="14">
-        <v>1</v>
-      </c>
-      <c r="P55" s="14">
-        <v>1</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -3960,17 +3983,14 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="C56" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D56" t="s">
         <v>7</v>
       </c>
-      <c r="E56" t="s">
-        <v>7</v>
-      </c>
       <c r="F56" t="s">
         <v>7</v>
       </c>
@@ -3978,19 +3998,10 @@
         <v>7</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="J56" t="s">
-        <v>180</v>
-      </c>
-      <c r="O56" s="14">
-        <v>1</v>
-      </c>
-      <c r="P56" s="14">
-        <v>2</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -3998,10 +4009,10 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="C57" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -4016,16 +4027,13 @@
         <v>7</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>190</v>
+        <v>80</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="O57" s="14">
-        <v>2</v>
-      </c>
-      <c r="P57" s="14">
-        <v>1</v>
+        <v>81</v>
+      </c>
+      <c r="J57" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -4033,10 +4041,10 @@
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="C58" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="D58" t="s">
         <v>7</v>
@@ -4051,16 +4059,10 @@
         <v>7</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="O58" s="14">
-        <v>2</v>
-      </c>
-      <c r="P58" s="14">
-        <v>2</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -4068,10 +4070,10 @@
         <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C59" t="s">
-        <v>183</v>
+        <v>111</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -4086,16 +4088,16 @@
         <v>7</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>192</v>
+        <v>127</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>183</v>
+        <v>111</v>
       </c>
       <c r="O59" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P59" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -4103,10 +4105,10 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C60" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
@@ -4121,16 +4123,19 @@
         <v>7</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>193</v>
+        <v>155</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>184</v>
+        <v>164</v>
+      </c>
+      <c r="J60" t="s">
+        <v>176</v>
       </c>
       <c r="O60" s="14">
         <v>1</v>
       </c>
       <c r="P60" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -4138,10 +4143,10 @@
         <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C61" t="s">
-        <v>86</v>
+        <v>177</v>
       </c>
       <c r="D61" t="s">
         <v>7</v>
@@ -4156,13 +4161,13 @@
         <v>7</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>86</v>
+        <v>177</v>
       </c>
       <c r="O61" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P61" s="14">
         <v>1</v>
@@ -4173,10 +4178,10 @@
         <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C62" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
@@ -4191,13 +4196,13 @@
         <v>7</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="O62" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P62" s="14">
         <v>2</v>
@@ -4208,14 +4213,17 @@
         <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C63" t="s">
-        <v>88</v>
+        <v>179</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
       </c>
+      <c r="E63" t="s">
+        <v>7</v>
+      </c>
       <c r="F63" t="s">
         <v>7</v>
       </c>
@@ -4223,13 +4231,13 @@
         <v>7</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>93</v>
+        <v>188</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>94</v>
+        <v>179</v>
       </c>
       <c r="O63" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P63" s="14">
         <v>3</v>
@@ -4240,10 +4248,10 @@
         <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C64" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="D64" t="s">
         <v>7</v>
@@ -4254,14 +4262,17 @@
       <c r="F64" t="s">
         <v>7</v>
       </c>
+      <c r="G64" t="s">
+        <v>7</v>
+      </c>
       <c r="H64" s="7" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="O64" s="14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P64" s="14">
         <v>3</v>
@@ -4272,10 +4283,10 @@
         <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C65" t="s">
-        <v>185</v>
+        <v>86</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
@@ -4286,17 +4297,20 @@
       <c r="F65" t="s">
         <v>7</v>
       </c>
+      <c r="G65" t="s">
+        <v>7</v>
+      </c>
       <c r="H65" s="7" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="I65" s="7" t="s">
-        <v>196</v>
+        <v>86</v>
       </c>
       <c r="O65" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P65" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
@@ -4304,28 +4318,34 @@
         <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C66" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
       </c>
+      <c r="E66" t="s">
+        <v>7</v>
+      </c>
       <c r="F66" t="s">
         <v>7</v>
       </c>
+      <c r="G66" t="s">
+        <v>7</v>
+      </c>
       <c r="H66" s="7" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="O66" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P66" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -4333,10 +4353,10 @@
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C67" t="s">
-        <v>187</v>
+        <v>88</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
@@ -4344,17 +4364,20 @@
       <c r="F67" t="s">
         <v>7</v>
       </c>
+      <c r="G67" t="s">
+        <v>7</v>
+      </c>
       <c r="H67" s="7" t="s">
-        <v>202</v>
+        <v>93</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>199</v>
+        <v>94</v>
       </c>
       <c r="O67" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P67" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
@@ -4362,28 +4385,31 @@
         <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C68" t="s">
-        <v>188</v>
+        <v>219</v>
       </c>
       <c r="D68" t="s">
         <v>7</v>
       </c>
+      <c r="E68" t="s">
+        <v>7</v>
+      </c>
       <c r="F68" t="s">
         <v>7</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="O68" s="14">
         <v>4</v>
       </c>
       <c r="P68" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
@@ -4391,28 +4417,31 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C69" t="s">
-        <v>124</v>
+        <v>181</v>
       </c>
       <c r="D69" t="s">
         <v>7</v>
       </c>
+      <c r="E69" t="s">
+        <v>7</v>
+      </c>
       <c r="F69" t="s">
         <v>7</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>143</v>
+        <v>191</v>
       </c>
       <c r="I69" s="7" t="s">
-        <v>124</v>
+        <v>192</v>
       </c>
       <c r="O69" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P69" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
@@ -4420,10 +4449,10 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C70" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D70" t="s">
         <v>7</v>
@@ -4431,14 +4460,17 @@
       <c r="F70" t="s">
         <v>7</v>
       </c>
-      <c r="G70" t="s">
-        <v>7</v>
-      </c>
       <c r="H70" s="7" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="I70" s="7" t="s">
-        <v>176</v>
+        <v>194</v>
+      </c>
+      <c r="O70" s="14">
+        <v>4</v>
+      </c>
+      <c r="P70" s="14">
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
@@ -4446,31 +4478,28 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C71" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="D71" t="s">
         <v>7</v>
       </c>
-      <c r="E71" t="s">
-        <v>7</v>
-      </c>
       <c r="F71" t="s">
         <v>7</v>
       </c>
-      <c r="G71" t="s">
-        <v>7</v>
-      </c>
       <c r="H71" s="7" t="s">
-        <v>80</v>
+        <v>198</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="J71" t="s">
-        <v>169</v>
+        <v>195</v>
+      </c>
+      <c r="O71" s="14">
+        <v>5</v>
+      </c>
+      <c r="P71" s="14">
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
@@ -4478,28 +4507,144 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C72" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
       </c>
-      <c r="E72" t="s">
-        <v>7</v>
-      </c>
       <c r="F72" t="s">
         <v>7</v>
       </c>
-      <c r="G72" t="s">
-        <v>7</v>
-      </c>
       <c r="H72" s="7" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="I72" s="7" t="s">
-        <v>170</v>
+        <v>196</v>
+      </c>
+      <c r="O72" s="14">
+        <v>4</v>
+      </c>
+      <c r="P72" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73" t="s">
+        <v>168</v>
+      </c>
+      <c r="C73" t="s">
+        <v>124</v>
+      </c>
+      <c r="D73" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" t="s">
+        <v>7</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="O73" s="14">
+        <v>5</v>
+      </c>
+      <c r="P73" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74" t="s">
+        <v>169</v>
+      </c>
+      <c r="C74" t="s">
+        <v>185</v>
+      </c>
+      <c r="D74" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" t="s">
+        <v>7</v>
+      </c>
+      <c r="G74" t="s">
+        <v>7</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="I74" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75" t="s">
+        <v>169</v>
+      </c>
+      <c r="C75" t="s">
+        <v>163</v>
+      </c>
+      <c r="D75" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" t="s">
+        <v>7</v>
+      </c>
+      <c r="G75" t="s">
+        <v>7</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J75" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>11</v>
+      </c>
+      <c r="B76" t="s">
+        <v>169</v>
+      </c>
+      <c r="C76" t="s">
+        <v>166</v>
+      </c>
+      <c r="D76" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76" t="s">
+        <v>7</v>
+      </c>
+      <c r="G76" t="s">
+        <v>7</v>
+      </c>
+      <c r="H76" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I76" s="7" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -4592,7 +4737,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
container min price and position payment type
</commit_message>
<xml_diff>
--- a/ContainerStar/ContainerStar/Generation/ContainerStar.Generation/Declarations/Stammdaten.xlsx
+++ b/ContainerStar/ContainerStar/Generation/ContainerStar.Generation/Declarations/Stammdaten.xlsx
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="249">
   <si>
     <t>Schema</t>
   </si>
@@ -893,6 +893,9 @@
   </si>
   <si>
     <t>Min Preis</t>
+  </si>
+  <si>
+    <t>MinPrice</t>
   </si>
 </sst>
 </file>
@@ -2334,10 +2337,10 @@
   <dimension ref="A1:R78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H67" sqref="H67"/>
+      <selection pane="bottomRight" activeCell="O70" sqref="O70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4318,7 +4321,7 @@
         <v>168</v>
       </c>
       <c r="C66" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
@@ -4342,7 +4345,7 @@
         <v>3</v>
       </c>
       <c r="P66" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -4441,7 +4444,7 @@
         <v>94</v>
       </c>
       <c r="O69" s="14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P69" s="14">
         <v>3</v>
@@ -4473,7 +4476,7 @@
         <v>221</v>
       </c>
       <c r="O70" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P70" s="14">
         <v>3</v>
@@ -4505,7 +4508,7 @@
         <v>192</v>
       </c>
       <c r="O71" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P71" s="14">
         <v>3</v>

</xml_diff>